<commit_message>
Updates in τ and θ
</commit_message>
<xml_diff>
--- a/ColorTransfer/Test/PD-Critical.xlsx
+++ b/ColorTransfer/Test/PD-Critical.xlsx
@@ -389,7 +389,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -423,19 +423,19 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0.02744798902934886</v>
+        <v>0.009122927242422047</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2">
-        <v>0.5159205722746036</v>
+        <v>0.8391058305229562</v>
       </c>
       <c r="F2">
-        <v>0.001525402069091797</v>
+        <v>0.001183986663818359</v>
       </c>
       <c r="G2">
-        <v>0.9943514917398668</v>
+        <v>0.9923652692346242</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -443,22 +443,22 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C3">
-        <v>0.05418734605623229</v>
+        <v>0.05130013785025216</v>
       </c>
       <c r="D3">
         <v>0.1</v>
       </c>
       <c r="E3">
-        <v>0.0443387513449028</v>
+        <v>0.09525825931251762</v>
       </c>
       <c r="F3">
-        <v>0.00440216064453125</v>
+        <v>0.004054069519042969</v>
       </c>
       <c r="G3">
-        <v>0.9794267526079573</v>
+        <v>0.9671611762514712</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -466,22 +466,22 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="C4">
-        <v>0.05663861903995152</v>
+        <v>0.05643587430324096</v>
       </c>
       <c r="D4">
         <v>0.01</v>
       </c>
       <c r="E4">
-        <v>0.001107503260070882</v>
+        <v>0.004683158876088452</v>
       </c>
       <c r="F4">
-        <v>0.005245208740234375</v>
+        <v>0.006312370300292969</v>
       </c>
       <c r="G4">
-        <v>0.975986304295077</v>
+        <v>0.9390188645614022</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -489,22 +489,22 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>1885</v>
+        <v>95</v>
       </c>
       <c r="C5">
-        <v>0.05675808151671367</v>
+        <v>0.05672714649778521</v>
       </c>
       <c r="D5">
         <v>0.001</v>
       </c>
       <c r="E5">
-        <v>0.0009993661110823124</v>
+        <v>0.0004537885737423669</v>
       </c>
       <c r="F5">
-        <v>1.387076139450073</v>
+        <v>0.02941203117370605</v>
       </c>
       <c r="G5">
-        <v>0.6270688390500064</v>
+        <v>0.8513239876363956</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -512,22 +512,22 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>10665</v>
+        <v>115</v>
       </c>
       <c r="C6">
-        <v>0.05670706331823926</v>
+        <v>0.05669951160987683</v>
       </c>
       <c r="D6">
         <v>0.0001</v>
       </c>
       <c r="E6">
-        <v>9.959672197821181E-05</v>
+        <v>3.358704818894733E-05</v>
       </c>
       <c r="F6">
-        <v>7.606749296188354</v>
+        <v>0.03550863265991211</v>
       </c>
       <c r="G6">
-        <v>0.3707229844828139</v>
+        <v>0.8383301384878855</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -535,22 +535,22 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>43163</v>
+        <v>312</v>
       </c>
       <c r="C7">
-        <v>0.05670198295619715</v>
+        <v>0.05670125280906785</v>
       </c>
       <c r="D7">
         <v>1E-05</v>
       </c>
       <c r="E7">
-        <v>9.998218155129855E-06</v>
+        <v>2.878834664001203E-06</v>
       </c>
       <c r="F7">
-        <v>32.196622133255</v>
+        <v>0.09159636497497559</v>
       </c>
       <c r="G7">
-        <v>0.1780661659360412</v>
+        <v>0.753448562284518</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -558,22 +558,45 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>81938</v>
+        <v>594</v>
       </c>
       <c r="C8">
-        <v>0.05670147217535223</v>
+        <v>0.05670139881194544</v>
       </c>
       <c r="D8">
         <v>1E-06</v>
       </c>
       <c r="E8">
-        <v>9.899626198953622E-07</v>
+        <v>3.038923118988512E-07</v>
       </c>
       <c r="F8">
-        <v>61.56228828430176</v>
+        <v>0.1734015941619873</v>
       </c>
       <c r="G8">
-        <v>0.1115551499826239</v>
+        <v>0.6844855791674191</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>3198</v>
+      </c>
+      <c r="C9">
+        <v>0.05670141636398267</v>
+      </c>
+      <c r="D9">
+        <v>1E-07</v>
+      </c>
+      <c r="E9">
+        <v>5.659696698042492E-09</v>
+      </c>
+      <c r="F9">
+        <v>0.950007438659668</v>
+      </c>
+      <c r="G9">
+        <v>0.4519505583416418</v>
       </c>
     </row>
   </sheetData>

</xml_diff>